<commit_message>
Version of the three computers were merged.
</commit_message>
<xml_diff>
--- a/PaperNeural/ExperimentsConfigMar2017_23-Mar-2017_pcbiolab.xlsx
+++ b/PaperNeural/ExperimentsConfigMar2017_23-Mar-2017_pcbiolab.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4529" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4572" uniqueCount="472">
   <si>
     <t>WorkFolder</t>
   </si>
@@ -1381,6 +1381,75 @@
   </si>
   <si>
     <t>T3_Supination and pronation_Sammon_FS-IF-IA_05-Apr-2017_MI_3000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T3_Supination and pronation_Sammon_FS-IF-IA_06-Apr-2017_MI_3000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T4_Rest_Sammon_FS_06-Apr-2017_MI_3000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T4_Rest_Sammon_IF_06-Apr-2017_MI_3000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T4_Rest_Sammon_IA_06-Apr-2017_MI_3000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T4_Rest_Sammon_FS-IF_06-Apr-2017_MI_3000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T4_Rest_Sammon_FS-IA_06-Apr-2017_MI_3000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T4_Rest_Sammon_IF-IA_06-Apr-2017_MI_3000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T4_Rest_Sammon_FS-IF-IA_06-Apr-2017_MI_3000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T1_Finger taps_Sammon_FS_06-Apr-2017_MI_4000_LR_0.5</t>
+  </si>
+  <si>
+    <t>ResultsMar2017-Sammon_MI_4000_LR_0.5.xlsx</t>
+  </si>
+  <si>
+    <t>T1_Finger taps_Sammon_IF_06-Apr-2017_MI_4000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T1_Finger taps_Sammon_IA_06-Apr-2017_MI_4000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T1_Finger taps_Sammon_FS-IF_06-Apr-2017_MI_4000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T1_Finger taps_Sammon_FS-IA_06-Apr-2017_MI_4000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T1_Finger taps_Sammon_IF-IA_06-Apr-2017_MI_4000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T1_Finger taps_Sammon_FS-IF-IA_06-Apr-2017_MI_4000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T2_Finger to nose_Sammon_FS_06-Apr-2017_MI_4000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T2_Finger to nose_Sammon_IF_06-Apr-2017_MI_4000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T2_Finger to nose_Sammon_IA_06-Apr-2017_MI_4000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T2_Finger to nose_Sammon_FS-IF_06-Apr-2017_MI_4000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T2_Finger to nose_Sammon_FS-IA_06-Apr-2017_MI_4000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T2_Finger to nose_Sammon_IF-IA_06-Apr-2017_MI_4000_LR_0.5</t>
+  </si>
+  <si>
+    <t>T2_Finger to nose_Sammon_FS-IF-IA_06-Apr-2017_MI_4000_LR_0.5</t>
   </si>
 </sst>
 </file>
@@ -26940,17 +27009,29 @@
       <c r="M386" t="s">
         <v>4</v>
       </c>
-      <c r="N386">
-        <v>0</v>
+      <c r="N386" t="n">
+        <v>1.0</v>
       </c>
       <c r="O386" t="n">
-        <v>863.0</v>
+        <v>387.0</v>
       </c>
       <c r="P386" t="n">
-        <v>0.04502060899527347</v>
+        <v>0.04396420463444639</v>
+      </c>
+      <c r="Q386" t="n">
+        <v>17.238508626221513</v>
+      </c>
+      <c r="R386" t="n">
+        <v>77.19298245614036</v>
+      </c>
+      <c r="S386" t="n">
+        <v>73.6842105263158</v>
       </c>
       <c r="T386" t="s">
-        <v>448</v>
+        <v>449</v>
+      </c>
+      <c r="U386" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="387" spans="1:14" x14ac:dyDescent="0.2">
@@ -26993,8 +27074,29 @@
       <c r="M387" t="s">
         <v>4</v>
       </c>
-      <c r="N387">
-        <v>0</v>
+      <c r="N387" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O387" t="n">
+        <v>561.0</v>
+      </c>
+      <c r="P387" t="n">
+        <v>0.025518751723765307</v>
+      </c>
+      <c r="Q387" t="n">
+        <v>7.450914789672176</v>
+      </c>
+      <c r="R387" t="n">
+        <v>68.42105263157895</v>
+      </c>
+      <c r="S387" t="n">
+        <v>63.15789473684212</v>
+      </c>
+      <c r="T387" t="s">
+        <v>450</v>
+      </c>
+      <c r="U387" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="388" spans="1:14" x14ac:dyDescent="0.2">
@@ -27037,8 +27139,29 @@
       <c r="M388" t="s">
         <v>4</v>
       </c>
-      <c r="N388">
-        <v>0</v>
+      <c r="N388" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O388" t="n">
+        <v>467.0</v>
+      </c>
+      <c r="P388" t="n">
+        <v>0.04743784469949855</v>
+      </c>
+      <c r="Q388" t="n">
+        <v>17.747292084363693</v>
+      </c>
+      <c r="R388" t="n">
+        <v>70.17543859649123</v>
+      </c>
+      <c r="S388" t="n">
+        <v>78.94736842105263</v>
+      </c>
+      <c r="T388" t="s">
+        <v>451</v>
+      </c>
+      <c r="U388" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="389" spans="1:14" x14ac:dyDescent="0.2">
@@ -27081,8 +27204,29 @@
       <c r="M389" t="s">
         <v>4</v>
       </c>
-      <c r="N389">
-        <v>0</v>
+      <c r="N389" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O389" t="n">
+        <v>348.0</v>
+      </c>
+      <c r="P389" t="n">
+        <v>0.02871769084791272</v>
+      </c>
+      <c r="Q389" t="n">
+        <v>29.386682582976263</v>
+      </c>
+      <c r="R389" t="n">
+        <v>67.83625730994152</v>
+      </c>
+      <c r="S389" t="n">
+        <v>78.94736842105263</v>
+      </c>
+      <c r="T389" t="s">
+        <v>452</v>
+      </c>
+      <c r="U389" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="390" spans="1:14" x14ac:dyDescent="0.2">
@@ -27125,8 +27269,29 @@
       <c r="M390" t="s">
         <v>4</v>
       </c>
-      <c r="N390">
-        <v>0</v>
+      <c r="N390" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O390" t="n">
+        <v>3000.0</v>
+      </c>
+      <c r="P390" t="n">
+        <v>0.040678362939114684</v>
+      </c>
+      <c r="Q390" t="n">
+        <v>21.370258284066885</v>
+      </c>
+      <c r="R390" t="n">
+        <v>77.77777777777777</v>
+      </c>
+      <c r="S390" t="n">
+        <v>78.94736842105263</v>
+      </c>
+      <c r="T390" t="s">
+        <v>453</v>
+      </c>
+      <c r="U390" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="391" spans="1:14" x14ac:dyDescent="0.2">
@@ -27169,8 +27334,29 @@
       <c r="M391" t="s">
         <v>4</v>
       </c>
-      <c r="N391">
-        <v>0</v>
+      <c r="N391" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O391" t="n">
+        <v>495.0</v>
+      </c>
+      <c r="P391" t="n">
+        <v>0.028080396363575802</v>
+      </c>
+      <c r="Q391" t="n">
+        <v>17.439436136485227</v>
+      </c>
+      <c r="R391" t="n">
+        <v>70.76023391812865</v>
+      </c>
+      <c r="S391" t="n">
+        <v>73.6842105263158</v>
+      </c>
+      <c r="T391" t="s">
+        <v>454</v>
+      </c>
+      <c r="U391" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="392" spans="1:14" x14ac:dyDescent="0.2">
@@ -27213,8 +27399,29 @@
       <c r="M392" t="s">
         <v>4</v>
       </c>
-      <c r="N392">
-        <v>0</v>
+      <c r="N392" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O392" t="n">
+        <v>1021.0</v>
+      </c>
+      <c r="P392" t="n">
+        <v>0.043332922454232536</v>
+      </c>
+      <c r="Q392" t="n">
+        <v>27.819165346437043</v>
+      </c>
+      <c r="R392" t="n">
+        <v>75.43859649122807</v>
+      </c>
+      <c r="S392" t="n">
+        <v>78.94736842105263</v>
+      </c>
+      <c r="T392" t="s">
+        <v>455</v>
+      </c>
+      <c r="U392" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="393" spans="1:14" x14ac:dyDescent="0.2">
@@ -27257,8 +27464,29 @@
       <c r="M393" t="s">
         <v>4</v>
       </c>
-      <c r="N393">
-        <v>0</v>
+      <c r="N393" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O393" t="n">
+        <v>826.0</v>
+      </c>
+      <c r="P393" t="n">
+        <v>0.040010344537007976</v>
+      </c>
+      <c r="Q393" t="n">
+        <v>23.456215257883798</v>
+      </c>
+      <c r="R393" t="n">
+        <v>75.43859649122807</v>
+      </c>
+      <c r="S393" t="n">
+        <v>78.94736842105263</v>
+      </c>
+      <c r="T393" t="s">
+        <v>456</v>
+      </c>
+      <c r="U393" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="394" spans="1:14" x14ac:dyDescent="0.2">
@@ -27301,8 +27529,29 @@
       <c r="M394" t="s">
         <v>4</v>
       </c>
-      <c r="N394">
-        <v>0</v>
+      <c r="N394" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O394" t="n">
+        <v>386.0</v>
+      </c>
+      <c r="P394" t="n">
+        <v>0.033276475332387735</v>
+      </c>
+      <c r="Q394" t="n">
+        <v>7.492143424751974</v>
+      </c>
+      <c r="R394" t="n">
+        <v>85.38011695906432</v>
+      </c>
+      <c r="S394" t="n">
+        <v>68.42105263157896</v>
+      </c>
+      <c r="T394" t="s">
+        <v>457</v>
+      </c>
+      <c r="U394" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="395" spans="1:14" x14ac:dyDescent="0.2">
@@ -27345,8 +27594,29 @@
       <c r="M395" t="s">
         <v>4</v>
       </c>
-      <c r="N395">
-        <v>0</v>
+      <c r="N395" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O395" t="n">
+        <v>425.0</v>
+      </c>
+      <c r="P395" t="n">
+        <v>0.05297079079312436</v>
+      </c>
+      <c r="Q395" t="n">
+        <v>22.26747779750949</v>
+      </c>
+      <c r="R395" t="n">
+        <v>73.09941520467837</v>
+      </c>
+      <c r="S395" t="n">
+        <v>52.63157894736844</v>
+      </c>
+      <c r="T395" t="s">
+        <v>459</v>
+      </c>
+      <c r="U395" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="396" spans="1:14" x14ac:dyDescent="0.2">
@@ -27389,8 +27659,29 @@
       <c r="M396" t="s">
         <v>4</v>
       </c>
-      <c r="N396">
-        <v>0</v>
+      <c r="N396" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O396" t="n">
+        <v>543.0</v>
+      </c>
+      <c r="P396" t="n">
+        <v>0.03474891418136164</v>
+      </c>
+      <c r="Q396" t="n">
+        <v>6.934086693764326</v>
+      </c>
+      <c r="R396" t="n">
+        <v>78.94736842105263</v>
+      </c>
+      <c r="S396" t="n">
+        <v>68.42105263157896</v>
+      </c>
+      <c r="T396" t="s">
+        <v>460</v>
+      </c>
+      <c r="U396" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="397" spans="1:14" x14ac:dyDescent="0.2">
@@ -27433,8 +27724,29 @@
       <c r="M397" t="s">
         <v>4</v>
       </c>
-      <c r="N397">
-        <v>0</v>
+      <c r="N397" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O397" t="n">
+        <v>1461.0</v>
+      </c>
+      <c r="P397" t="n">
+        <v>0.04757995748830339</v>
+      </c>
+      <c r="Q397" t="n">
+        <v>38.79562766488739</v>
+      </c>
+      <c r="R397" t="n">
+        <v>80.11695906432749</v>
+      </c>
+      <c r="S397" t="n">
+        <v>68.42105263157896</v>
+      </c>
+      <c r="T397" t="s">
+        <v>461</v>
+      </c>
+      <c r="U397" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="398" spans="1:14" x14ac:dyDescent="0.2">
@@ -27477,8 +27789,29 @@
       <c r="M398" t="s">
         <v>4</v>
       </c>
-      <c r="N398">
-        <v>0</v>
+      <c r="N398" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O398" t="n">
+        <v>668.0</v>
+      </c>
+      <c r="P398" t="n">
+        <v>0.035779420904758184</v>
+      </c>
+      <c r="Q398" t="n">
+        <v>10.651671977948329</v>
+      </c>
+      <c r="R398" t="n">
+        <v>81.28654970760233</v>
+      </c>
+      <c r="S398" t="n">
+        <v>73.6842105263158</v>
+      </c>
+      <c r="T398" t="s">
+        <v>462</v>
+      </c>
+      <c r="U398" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="399" spans="1:14" x14ac:dyDescent="0.2">
@@ -27521,8 +27854,29 @@
       <c r="M399" t="s">
         <v>4</v>
       </c>
-      <c r="N399">
-        <v>0</v>
+      <c r="N399" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O399" t="n">
+        <v>1902.0</v>
+      </c>
+      <c r="P399" t="n">
+        <v>0.04852974848121782</v>
+      </c>
+      <c r="Q399" t="n">
+        <v>17.63774121897484</v>
+      </c>
+      <c r="R399" t="n">
+        <v>80.11695906432749</v>
+      </c>
+      <c r="S399" t="n">
+        <v>63.15789473684212</v>
+      </c>
+      <c r="T399" t="s">
+        <v>463</v>
+      </c>
+      <c r="U399" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="400" spans="1:14" x14ac:dyDescent="0.2">
@@ -27565,8 +27919,29 @@
       <c r="M400" t="s">
         <v>4</v>
       </c>
-      <c r="N400">
-        <v>0</v>
+      <c r="N400" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O400" t="n">
+        <v>567.0</v>
+      </c>
+      <c r="P400" t="n">
+        <v>0.04470052095758281</v>
+      </c>
+      <c r="Q400" t="n">
+        <v>34.20937973731283</v>
+      </c>
+      <c r="R400" t="n">
+        <v>81.28654970760233</v>
+      </c>
+      <c r="S400" t="n">
+        <v>84.21052631578948</v>
+      </c>
+      <c r="T400" t="s">
+        <v>464</v>
+      </c>
+      <c r="U400" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="401" spans="1:14" x14ac:dyDescent="0.2">
@@ -27609,8 +27984,29 @@
       <c r="M401" t="s">
         <v>4</v>
       </c>
-      <c r="N401">
-        <v>0</v>
+      <c r="N401" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O401" t="n">
+        <v>359.0</v>
+      </c>
+      <c r="P401" t="n">
+        <v>0.03623810463778771</v>
+      </c>
+      <c r="Q401" t="n">
+        <v>3.6522599069320476</v>
+      </c>
+      <c r="R401" t="n">
+        <v>80.11695906432749</v>
+      </c>
+      <c r="S401" t="n">
+        <v>73.6842105263158</v>
+      </c>
+      <c r="T401" t="s">
+        <v>465</v>
+      </c>
+      <c r="U401" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="402" spans="1:14" x14ac:dyDescent="0.2">
@@ -27653,8 +28049,29 @@
       <c r="M402" t="s">
         <v>4</v>
       </c>
-      <c r="N402">
-        <v>0</v>
+      <c r="N402" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O402" t="n">
+        <v>577.0</v>
+      </c>
+      <c r="P402" t="n">
+        <v>0.05189347750460582</v>
+      </c>
+      <c r="Q402" t="n">
+        <v>17.2051003349763</v>
+      </c>
+      <c r="R402" t="n">
+        <v>77.19298245614036</v>
+      </c>
+      <c r="S402" t="n">
+        <v>73.6842105263158</v>
+      </c>
+      <c r="T402" t="s">
+        <v>466</v>
+      </c>
+      <c r="U402" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="403" spans="1:14" x14ac:dyDescent="0.2">
@@ -27697,8 +28114,29 @@
       <c r="M403" t="s">
         <v>4</v>
       </c>
-      <c r="N403">
-        <v>0</v>
+      <c r="N403" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O403" t="n">
+        <v>399.0</v>
+      </c>
+      <c r="P403" t="n">
+        <v>0.035121183484197536</v>
+      </c>
+      <c r="Q403" t="n">
+        <v>7.0167752252638085</v>
+      </c>
+      <c r="R403" t="n">
+        <v>75.43859649122807</v>
+      </c>
+      <c r="S403" t="n">
+        <v>68.42105263157896</v>
+      </c>
+      <c r="T403" t="s">
+        <v>467</v>
+      </c>
+      <c r="U403" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="404" spans="1:14" x14ac:dyDescent="0.2">
@@ -27741,8 +28179,29 @@
       <c r="M404" t="s">
         <v>4</v>
       </c>
-      <c r="N404">
-        <v>0</v>
+      <c r="N404" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O404" t="n">
+        <v>351.0</v>
+      </c>
+      <c r="P404" t="n">
+        <v>0.04867543591896745</v>
+      </c>
+      <c r="Q404" t="n">
+        <v>21.371173527575458</v>
+      </c>
+      <c r="R404" t="n">
+        <v>85.96491228070175</v>
+      </c>
+      <c r="S404" t="n">
+        <v>84.21052631578948</v>
+      </c>
+      <c r="T404" t="s">
+        <v>468</v>
+      </c>
+      <c r="U404" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="405" spans="1:14" x14ac:dyDescent="0.2">
@@ -27785,8 +28244,29 @@
       <c r="M405" t="s">
         <v>4</v>
       </c>
-      <c r="N405">
-        <v>0</v>
+      <c r="N405" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O405" t="n">
+        <v>491.0</v>
+      </c>
+      <c r="P405" t="n">
+        <v>0.03865048214386203</v>
+      </c>
+      <c r="Q405" t="n">
+        <v>7.9605961691835</v>
+      </c>
+      <c r="R405" t="n">
+        <v>70.17543859649123</v>
+      </c>
+      <c r="S405" t="n">
+        <v>84.21052631578948</v>
+      </c>
+      <c r="T405" t="s">
+        <v>469</v>
+      </c>
+      <c r="U405" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="406" spans="1:14" x14ac:dyDescent="0.2">
@@ -27829,8 +28309,29 @@
       <c r="M406" t="s">
         <v>4</v>
       </c>
-      <c r="N406">
-        <v>0</v>
+      <c r="N406" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O406" t="n">
+        <v>509.0</v>
+      </c>
+      <c r="P406" t="n">
+        <v>0.048787228405706685</v>
+      </c>
+      <c r="Q406" t="n">
+        <v>21.24894109137171</v>
+      </c>
+      <c r="R406" t="n">
+        <v>87.71929824561404</v>
+      </c>
+      <c r="S406" t="n">
+        <v>68.42105263157896</v>
+      </c>
+      <c r="T406" t="s">
+        <v>470</v>
+      </c>
+      <c r="U406" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="407" spans="1:14" x14ac:dyDescent="0.2">
@@ -27875,6 +28376,15 @@
       </c>
       <c r="N407">
         <v>0</v>
+      </c>
+      <c r="O407" t="n">
+        <v>371.0</v>
+      </c>
+      <c r="P407" t="n">
+        <v>0.04789382389439819</v>
+      </c>
+      <c r="T407" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="408" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>